<commit_message>
Initial code to make a parellel coordinate plot
</commit_message>
<xml_diff>
--- a/sccp/data/ScibMetrics.xlsx
+++ b/sccp/data/ScibMetrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewramirezmacbook/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C008E987-9918-E640-9A51-18BF9D1301F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC6BE79-4612-774D-9A3C-BEE2DBE05A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="immune_cell_hum" sheetId="1" r:id="rId1"/>
@@ -22620,7 +22620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="A70" sqref="A70:A74"/>
     </sheetView>
   </sheetViews>
@@ -27608,7 +27608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
@@ -36722,11 +36722,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E11"/>
+    <sheetView topLeftCell="C58" zoomScale="111" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -41294,37 +41297,37 @@
       <c r="E71" t="s">
         <v>29</v>
       </c>
-      <c r="G71" s="3">
+      <c r="H71" s="3">
         <v>0.95904355154026599</v>
       </c>
-      <c r="H71" s="3">
+      <c r="I71" s="3">
         <v>0.81982060912417098</v>
       </c>
-      <c r="I71" s="3">
+      <c r="J71" s="3">
         <v>0.28435278862317498</v>
       </c>
-      <c r="J71" s="3">
+      <c r="K71" s="3">
         <v>0.57343399978807796</v>
       </c>
-      <c r="K71" s="3">
+      <c r="L71" s="3">
         <v>0.129823234928027</v>
       </c>
-      <c r="M71" s="3">
+      <c r="N71" s="3">
         <v>0.372667866855868</v>
       </c>
-      <c r="N71" s="3">
+      <c r="O71" s="3">
         <v>0.27991726002061701</v>
       </c>
-      <c r="O71" s="3">
+      <c r="P71" s="3">
         <v>0.45399440155215798</v>
-      </c>
-      <c r="P71" s="3">
-        <v>1.39372822299652E-2</v>
       </c>
       <c r="Q71" s="3">
         <v>1.39372822299652E-2</v>
       </c>
       <c r="R71" s="3">
+        <v>1.39372822299652E-2</v>
+      </c>
+      <c r="S71" s="3">
         <v>0.91770104949835896</v>
       </c>
     </row>
@@ -41344,37 +41347,37 @@
       <c r="E72" t="s">
         <v>29</v>
       </c>
-      <c r="G72" s="3">
+      <c r="H72" s="3">
         <v>0.98511845550196997</v>
       </c>
-      <c r="H72" s="3">
+      <c r="I72" s="3">
         <v>0.85145871185200295</v>
       </c>
-      <c r="I72" s="3">
+      <c r="J72" s="3">
         <v>0.33181731178538798</v>
       </c>
-      <c r="J72" s="3">
+      <c r="K72" s="3">
         <v>0.77890584381817396</v>
       </c>
-      <c r="K72" s="3">
+      <c r="L72" s="3">
         <v>0.26133270253796498</v>
       </c>
-      <c r="M72" s="3">
+      <c r="N72" s="3">
         <v>0.68334913807933395</v>
       </c>
-      <c r="N72" s="3">
+      <c r="O72" s="3">
         <v>0.71384856173637001</v>
       </c>
-      <c r="O72" s="3">
+      <c r="P72" s="3">
         <v>0.50633428427367999</v>
-      </c>
-      <c r="P72" s="3">
-        <v>6.5573770491803296E-2</v>
       </c>
       <c r="Q72" s="3">
         <v>6.5573770491803296E-2</v>
       </c>
       <c r="R72" s="3">
+        <v>6.5573770491803296E-2</v>
+      </c>
+      <c r="S72" s="3">
         <v>0.97916982503780303</v>
       </c>
     </row>
@@ -41394,37 +41397,37 @@
       <c r="E73" t="s">
         <v>29</v>
       </c>
-      <c r="G73" s="3">
+      <c r="H73" s="3">
         <v>0.993897734815265</v>
       </c>
-      <c r="H73" s="3">
+      <c r="I73" s="3">
         <v>0.87708156521413205</v>
       </c>
-      <c r="I73" s="3">
+      <c r="J73" s="3">
         <v>0.35500797877873103</v>
       </c>
-      <c r="J73" s="3">
+      <c r="K73" s="3">
         <v>0.88316884406594698</v>
       </c>
-      <c r="K73" s="3">
+      <c r="L73" s="3">
         <v>0.281988113008732</v>
       </c>
-      <c r="M73" s="3">
+      <c r="N73" s="3">
         <v>0.78418814958610805</v>
       </c>
-      <c r="N73" s="3">
+      <c r="O73" s="3">
         <v>0.841711157883132</v>
       </c>
-      <c r="O73" s="3">
+      <c r="P73" s="3">
         <v>0.519425761871814</v>
-      </c>
-      <c r="P73" s="3">
-        <v>0.133333333333333</v>
       </c>
       <c r="Q73" s="3">
         <v>0.133333333333333</v>
       </c>
       <c r="R73" s="3">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="S73" s="3">
         <v>0.98850517372207602</v>
       </c>
     </row>
@@ -41444,37 +41447,37 @@
       <c r="E74" t="s">
         <v>29</v>
       </c>
-      <c r="G74" s="3">
+      <c r="H74" s="3">
         <v>0.99658948740506903</v>
       </c>
-      <c r="H74" s="3">
+      <c r="I74" s="3">
         <v>0.88638025407950405</v>
       </c>
-      <c r="I74" s="3">
+      <c r="J74" s="3">
         <v>0.31562564678609001</v>
       </c>
-      <c r="J74" s="3">
+      <c r="K74" s="3">
         <v>0.91773045430259703</v>
       </c>
-      <c r="K74" s="3">
+      <c r="L74" s="3">
         <v>0.30493826894133103</v>
       </c>
-      <c r="M74" s="3">
+      <c r="N74" s="3">
         <v>0.80719822322128199</v>
       </c>
-      <c r="N74" s="3">
+      <c r="O74" s="3">
         <v>0.83636680352081305</v>
       </c>
-      <c r="O74" s="3">
+      <c r="P74" s="3">
         <v>0.51345604573572201</v>
-      </c>
-      <c r="P74" s="3">
-        <v>8.5106382978723402E-2</v>
       </c>
       <c r="Q74" s="3">
         <v>8.5106382978723402E-2</v>
       </c>
       <c r="R74" s="3">
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="S74" s="3">
         <v>0.97641708663336302</v>
       </c>
     </row>
@@ -42942,7 +42945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Initial code to make a parellel coordinate plot (#140)
* Initial code to make a parellel coordinate plot

* Using parellel coordinate plots correctly

* Changign color palette

---------

Co-authored-by: Andrew Ramirez <aramirez@aretha.seas.ucla.edu>
</commit_message>
<xml_diff>
--- a/sccp/data/ScibMetrics.xlsx
+++ b/sccp/data/ScibMetrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewramirezmacbook/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C008E987-9918-E640-9A51-18BF9D1301F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC6BE79-4612-774D-9A3C-BEE2DBE05A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="immune_cell_hum" sheetId="1" r:id="rId1"/>
@@ -22620,7 +22620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="A70" sqref="A70:A74"/>
     </sheetView>
   </sheetViews>
@@ -27608,7 +27608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
@@ -36722,11 +36722,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E11"/>
+    <sheetView topLeftCell="C58" zoomScale="111" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -41294,37 +41297,37 @@
       <c r="E71" t="s">
         <v>29</v>
       </c>
-      <c r="G71" s="3">
+      <c r="H71" s="3">
         <v>0.95904355154026599</v>
       </c>
-      <c r="H71" s="3">
+      <c r="I71" s="3">
         <v>0.81982060912417098</v>
       </c>
-      <c r="I71" s="3">
+      <c r="J71" s="3">
         <v>0.28435278862317498</v>
       </c>
-      <c r="J71" s="3">
+      <c r="K71" s="3">
         <v>0.57343399978807796</v>
       </c>
-      <c r="K71" s="3">
+      <c r="L71" s="3">
         <v>0.129823234928027</v>
       </c>
-      <c r="M71" s="3">
+      <c r="N71" s="3">
         <v>0.372667866855868</v>
       </c>
-      <c r="N71" s="3">
+      <c r="O71" s="3">
         <v>0.27991726002061701</v>
       </c>
-      <c r="O71" s="3">
+      <c r="P71" s="3">
         <v>0.45399440155215798</v>
-      </c>
-      <c r="P71" s="3">
-        <v>1.39372822299652E-2</v>
       </c>
       <c r="Q71" s="3">
         <v>1.39372822299652E-2</v>
       </c>
       <c r="R71" s="3">
+        <v>1.39372822299652E-2</v>
+      </c>
+      <c r="S71" s="3">
         <v>0.91770104949835896</v>
       </c>
     </row>
@@ -41344,37 +41347,37 @@
       <c r="E72" t="s">
         <v>29</v>
       </c>
-      <c r="G72" s="3">
+      <c r="H72" s="3">
         <v>0.98511845550196997</v>
       </c>
-      <c r="H72" s="3">
+      <c r="I72" s="3">
         <v>0.85145871185200295</v>
       </c>
-      <c r="I72" s="3">
+      <c r="J72" s="3">
         <v>0.33181731178538798</v>
       </c>
-      <c r="J72" s="3">
+      <c r="K72" s="3">
         <v>0.77890584381817396</v>
       </c>
-      <c r="K72" s="3">
+      <c r="L72" s="3">
         <v>0.26133270253796498</v>
       </c>
-      <c r="M72" s="3">
+      <c r="N72" s="3">
         <v>0.68334913807933395</v>
       </c>
-      <c r="N72" s="3">
+      <c r="O72" s="3">
         <v>0.71384856173637001</v>
       </c>
-      <c r="O72" s="3">
+      <c r="P72" s="3">
         <v>0.50633428427367999</v>
-      </c>
-      <c r="P72" s="3">
-        <v>6.5573770491803296E-2</v>
       </c>
       <c r="Q72" s="3">
         <v>6.5573770491803296E-2</v>
       </c>
       <c r="R72" s="3">
+        <v>6.5573770491803296E-2</v>
+      </c>
+      <c r="S72" s="3">
         <v>0.97916982503780303</v>
       </c>
     </row>
@@ -41394,37 +41397,37 @@
       <c r="E73" t="s">
         <v>29</v>
       </c>
-      <c r="G73" s="3">
+      <c r="H73" s="3">
         <v>0.993897734815265</v>
       </c>
-      <c r="H73" s="3">
+      <c r="I73" s="3">
         <v>0.87708156521413205</v>
       </c>
-      <c r="I73" s="3">
+      <c r="J73" s="3">
         <v>0.35500797877873103</v>
       </c>
-      <c r="J73" s="3">
+      <c r="K73" s="3">
         <v>0.88316884406594698</v>
       </c>
-      <c r="K73" s="3">
+      <c r="L73" s="3">
         <v>0.281988113008732</v>
       </c>
-      <c r="M73" s="3">
+      <c r="N73" s="3">
         <v>0.78418814958610805</v>
       </c>
-      <c r="N73" s="3">
+      <c r="O73" s="3">
         <v>0.841711157883132</v>
       </c>
-      <c r="O73" s="3">
+      <c r="P73" s="3">
         <v>0.519425761871814</v>
-      </c>
-      <c r="P73" s="3">
-        <v>0.133333333333333</v>
       </c>
       <c r="Q73" s="3">
         <v>0.133333333333333</v>
       </c>
       <c r="R73" s="3">
+        <v>0.133333333333333</v>
+      </c>
+      <c r="S73" s="3">
         <v>0.98850517372207602</v>
       </c>
     </row>
@@ -41444,37 +41447,37 @@
       <c r="E74" t="s">
         <v>29</v>
       </c>
-      <c r="G74" s="3">
+      <c r="H74" s="3">
         <v>0.99658948740506903</v>
       </c>
-      <c r="H74" s="3">
+      <c r="I74" s="3">
         <v>0.88638025407950405</v>
       </c>
-      <c r="I74" s="3">
+      <c r="J74" s="3">
         <v>0.31562564678609001</v>
       </c>
-      <c r="J74" s="3">
+      <c r="K74" s="3">
         <v>0.91773045430259703</v>
       </c>
-      <c r="K74" s="3">
+      <c r="L74" s="3">
         <v>0.30493826894133103</v>
       </c>
-      <c r="M74" s="3">
+      <c r="N74" s="3">
         <v>0.80719822322128199</v>
       </c>
-      <c r="N74" s="3">
+      <c r="O74" s="3">
         <v>0.83636680352081305</v>
       </c>
-      <c r="O74" s="3">
+      <c r="P74" s="3">
         <v>0.51345604573572201</v>
-      </c>
-      <c r="P74" s="3">
-        <v>8.5106382978723402E-2</v>
       </c>
       <c r="Q74" s="3">
         <v>8.5106382978723402E-2</v>
       </c>
       <c r="R74" s="3">
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="S74" s="3">
         <v>0.97641708663336302</v>
       </c>
     </row>
@@ -42942,7 +42945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>